<commit_message>
Saved Booma's criteria for keeping potential matches
</commit_message>
<xml_diff>
--- a/docs/Matching Rules.xlsx
+++ b/docs/Matching Rules.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradcannell/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradcannell/Dropbox/01 Research/Elder Abuse/DETECT 2014-MU-CX-0102/r_proj_detect_pilot_1_year/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231E17CC-9B41-A24A-96B7-32D37C2F76B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892D7985-240D-234A-8D53-AA5C7A3944F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="1000" windowWidth="28040" windowHeight="17440" xr2:uid="{D4CB3254-7605-904E-9AA1-9BCE0040838E}"/>
+    <workbookView xWindow="38060" yWindow="2100" windowWidth="38080" windowHeight="23560" xr2:uid="{D4CB3254-7605-904E-9AA1-9BCE0040838E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="44">
   <si>
     <t>Rules for manually filtering potential matches</t>
   </si>
@@ -465,7 +464,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -564,7 +563,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -592,66 +591,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -977,11 +916,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C152FEC4-D35E-5B4A-AE10-F0FB0CF41B70}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="10" width="17" style="1" customWidth="1"/>
     <col min="11" max="11" width="28" style="2" bestFit="1" customWidth="1"/>
@@ -991,7 +930,7 @@
     <col min="17" max="17" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1">
+    <row r="1" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +950,7 @@
       <c r="O1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" s="7" customFormat="1">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1064,7 +1003,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1170,7 +1109,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1223,7 +1162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1276,7 +1215,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1329,7 +1268,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1365,12 +1304,6 @@
       </c>
       <c r="L8" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>18</v>

</xml_diff>